<commit_message>
Added test to iReadMore-testing.xlsx
</commit_message>
<xml_diff>
--- a/attachments/iReadMore-testing.xlsx
+++ b/attachments/iReadMore-testing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
   <si>
     <t>Testing of iReadMore WebApp</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Replaced smooth scrolling css style with JS, removed :hover pseudo class. Now works.</t>
+  </si>
+  <si>
+    <t>3. Selected contact icons in the footer</t>
   </si>
   <si>
     <t>Example values (appear when page is loaded)</t>
@@ -544,6 +547,21 @@
       <right style="thin">
         <color indexed="10"/>
       </right>
+      <top style="hair">
+        <color indexed="8"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -588,28 +606,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="hair">
-        <color indexed="8"/>
-      </top>
-      <bottom style="hair">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -661,6 +664,15 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -688,40 +700,37 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -733,10 +742,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1829,7 +1835,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1953,33 +1959,37 @@
       </c>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" t="s" s="17">
+      <c r="A8" s="17"/>
+      <c r="B8" t="s" s="18">
         <v>19</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="C8" t="s" s="18">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s" s="18">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s" s="18">
+        <v>13</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" t="s" s="19">
+      <c r="A9" t="s" s="20">
         <v>20</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="19">
+      <c r="A10" s="21"/>
+      <c r="B10" t="s" s="22">
         <v>21</v>
-      </c>
-      <c r="B10" t="s" s="19">
-        <v>22</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1988,34 +1998,30 @@
       <c r="G10" s="3"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" t="s" s="19">
+      <c r="A11" t="s" s="22">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s" s="22">
         <v>23</v>
       </c>
-      <c r="C11" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s" s="19">
-        <v>13</v>
-      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="13.65" customHeight="1">
       <c r="A12" s="3"/>
-      <c r="B12" t="s" s="19">
+      <c r="B12" t="s" s="22">
         <v>24</v>
       </c>
-      <c r="C12" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s" s="19">
+      <c r="C12" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F12" s="3"/>
@@ -2023,16 +2029,16 @@
     </row>
     <row r="13" ht="13.65" customHeight="1">
       <c r="A13" s="3"/>
-      <c r="B13" t="s" s="19">
+      <c r="B13" t="s" s="22">
         <v>25</v>
       </c>
-      <c r="C13" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E13" t="s" s="19">
+      <c r="C13" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F13" s="3"/>
@@ -2040,16 +2046,16 @@
     </row>
     <row r="14" ht="13.65" customHeight="1">
       <c r="A14" s="3"/>
-      <c r="B14" t="s" s="19">
+      <c r="B14" t="s" s="22">
         <v>26</v>
       </c>
-      <c r="C14" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s" s="19">
+      <c r="C14" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F14" s="3"/>
@@ -2057,16 +2063,16 @@
     </row>
     <row r="15" ht="13.65" customHeight="1">
       <c r="A15" s="3"/>
-      <c r="B15" t="s" s="19">
+      <c r="B15" t="s" s="22">
         <v>27</v>
       </c>
-      <c r="C15" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s" s="19">
+      <c r="C15" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D15" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E15" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F15" s="3"/>
@@ -2074,224 +2080,232 @@
     </row>
     <row r="16" ht="13.65" customHeight="1">
       <c r="A16" s="3"/>
-      <c r="B16" t="s" s="19">
+      <c r="B16" t="s" s="22">
         <v>28</v>
       </c>
-      <c r="C16" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s" s="19">
+      <c r="C16" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D16" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" s="14"/>
-      <c r="B17" t="s" s="15">
+      <c r="A17" s="3"/>
+      <c r="B17" t="s" s="22">
         <v>29</v>
       </c>
-      <c r="C17" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
+      <c r="C17" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D17" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
-      <c r="A18" t="s" s="12">
+      <c r="A18" s="14"/>
+      <c r="B18" t="s" s="15">
         <v>30</v>
       </c>
-      <c r="B18" t="s" s="12">
+      <c r="C18" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="D18" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" ht="13.65" customHeight="1">
+      <c r="A19" t="s" s="12">
         <v>31</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" ht="13.65" customHeight="1">
-      <c r="A19" s="3"/>
-      <c r="B19" t="s" s="19">
+      <c r="B19" t="s" s="12">
         <v>32</v>
       </c>
-      <c r="C19" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D19" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E19" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
     </row>
     <row r="20" ht="13.65" customHeight="1">
       <c r="A20" s="3"/>
-      <c r="B20" t="s" s="19">
+      <c r="B20" t="s" s="22">
         <v>33</v>
       </c>
-      <c r="C20" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D20" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E20" t="s" s="20">
+      <c r="C20" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" ht="13.65" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="B21" t="s" s="22">
         <v>34</v>
       </c>
-      <c r="F20" t="s" s="19">
+      <c r="C21" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D21" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s" s="23">
         <v>35</v>
       </c>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" ht="13.65" customHeight="1">
-      <c r="A21" s="14"/>
-      <c r="B21" t="s" s="15">
+      <c r="F21" t="s" s="22">
         <v>36</v>
       </c>
-      <c r="C21" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="D21" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" ht="13.65" customHeight="1">
-      <c r="A22" t="s" s="17">
+      <c r="A22" s="14"/>
+      <c r="B22" t="s" s="15">
         <v>37</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="C22" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
     </row>
     <row r="23" ht="13.65" customHeight="1">
-      <c r="A23" t="s" s="15">
+      <c r="A23" t="s" s="20">
         <v>38</v>
       </c>
-      <c r="B23" t="s" s="15">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" ht="13.65" customHeight="1">
+      <c r="A24" t="s" s="15">
         <v>39</v>
       </c>
-      <c r="C23" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s" s="16">
+      <c r="B24" t="s" s="15">
+        <v>40</v>
+      </c>
+      <c r="C24" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s" s="16">
         <v>16</v>
       </c>
-      <c r="E23" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="F23" t="s" s="15">
-        <v>40</v>
-      </c>
-      <c r="G23" t="s" s="21">
+      <c r="E24" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s" s="15">
         <v>41</v>
       </c>
-    </row>
-    <row r="24" ht="13.65" customHeight="1">
-      <c r="A24" t="s" s="12">
+      <c r="G24" t="s" s="24">
         <v>42</v>
       </c>
-      <c r="B24" t="s" s="12">
+    </row>
+    <row r="25" ht="13.65" customHeight="1">
+      <c r="A25" t="s" s="12">
         <v>43</v>
       </c>
-      <c r="C24" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="E24" t="s" s="22">
-        <v>34</v>
-      </c>
-      <c r="F24" t="s" s="12">
+      <c r="B25" t="s" s="12">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s" s="25">
         <v>35</v>
       </c>
-      <c r="G24" s="13"/>
-    </row>
-    <row r="25" ht="13.65" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" t="s" s="19">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E25" t="s" s="19">
-        <v>45</v>
-      </c>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="F25" t="s" s="12">
+        <v>36</v>
+      </c>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" ht="13.65" customHeight="1">
       <c r="A26" s="3"/>
-      <c r="B26" t="s" s="19">
+      <c r="B26" t="s" s="22">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s" s="22">
         <v>46</v>
-      </c>
-      <c r="C26" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D26" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s" s="19">
-        <v>45</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" ht="13.65" customHeight="1">
       <c r="A27" s="3"/>
-      <c r="B27" t="s" s="19">
+      <c r="B27" t="s" s="22">
         <v>47</v>
       </c>
-      <c r="C27" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D27" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E27" t="s" s="19">
-        <v>45</v>
+      <c r="C27" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E27" t="s" s="22">
+        <v>46</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" ht="13.65" customHeight="1">
       <c r="A28" s="3"/>
-      <c r="B28" t="s" s="19">
+      <c r="B28" t="s" s="22">
         <v>48</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="C28" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s" s="22">
+        <v>46</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" ht="13.65" customHeight="1">
       <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
+      <c r="B29" t="s" s="22">
+        <v>49</v>
+      </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -2299,9 +2313,7 @@
       <c r="G29" s="3"/>
     </row>
     <row r="30" ht="13.65" customHeight="1">
-      <c r="A30" t="s" s="23">
-        <v>49</v>
-      </c>
+      <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2310,37 +2322,37 @@
       <c r="G30" s="3"/>
     </row>
     <row r="31" ht="13.65" customHeight="1">
-      <c r="A31" t="s" s="19">
+      <c r="A31" t="s" s="26">
         <v>50</v>
       </c>
-      <c r="B31" t="s" s="19">
-        <v>51</v>
-      </c>
-      <c r="C31" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D31" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E31" t="s" s="19">
-        <v>13</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" ht="13.65" customHeight="1">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="A32" t="s" s="22">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s" s="22">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D32" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s" s="22">
+        <v>13</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" ht="13.65" customHeight="1">
-      <c r="A33" t="s" s="23">
-        <v>52</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -2349,136 +2361,136 @@
       <c r="G33" s="3"/>
     </row>
     <row r="34" ht="13.65" customHeight="1">
-      <c r="A34" t="s" s="19">
+      <c r="A34" t="s" s="26">
         <v>53</v>
       </c>
-      <c r="B34" t="s" s="19">
-        <v>54</v>
-      </c>
-      <c r="C34" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D34" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E34" t="s" s="19">
-        <v>13</v>
-      </c>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" ht="13.65" customHeight="1">
-      <c r="A35" t="s" s="19">
+      <c r="A35" t="s" s="22">
+        <v>54</v>
+      </c>
+      <c r="B35" t="s" s="22">
         <v>55</v>
       </c>
-      <c r="B35" t="s" s="19">
-        <v>56</v>
-      </c>
-      <c r="C35" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D35" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E35" t="s" s="19">
+      <c r="C35" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D35" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" ht="13.65" customHeight="1">
-      <c r="A36" t="s" s="19">
+      <c r="A36" t="s" s="22">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s" s="22">
         <v>57</v>
       </c>
-      <c r="B36" t="s" s="19">
-        <v>58</v>
-      </c>
-      <c r="C36" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D36" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E36" t="s" s="19">
+      <c r="C36" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D36" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
     </row>
     <row r="37" ht="13.65" customHeight="1">
-      <c r="A37" t="s" s="19">
+      <c r="A37" t="s" s="22">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s" s="22">
         <v>59</v>
       </c>
-      <c r="B37" t="s" s="19">
-        <v>60</v>
-      </c>
-      <c r="C37" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D37" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E37" t="s" s="19">
+      <c r="C37" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" ht="13.65" customHeight="1">
-      <c r="A38" t="s" s="19">
+      <c r="A38" t="s" s="22">
+        <v>60</v>
+      </c>
+      <c r="B38" t="s" s="22">
         <v>61</v>
       </c>
-      <c r="B38" t="s" s="19">
+      <c r="C38" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D38" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" ht="13.65" customHeight="1">
+      <c r="A39" t="s" s="22">
         <v>62</v>
       </c>
-      <c r="C38" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D38" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E38" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" t="s" s="24">
+      <c r="B39" t="s" s="22">
         <v>63</v>
       </c>
-    </row>
-    <row r="39" ht="13.65" customHeight="1">
-      <c r="A39" t="s" s="19">
+      <c r="C39" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="F39" s="3"/>
+      <c r="G39" t="s" s="27">
         <v>64</v>
       </c>
-      <c r="B39" t="s" s="19">
+    </row>
+    <row r="40" ht="13.65" customHeight="1">
+      <c r="A40" t="s" s="22">
         <v>65</v>
       </c>
-      <c r="C39" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D39" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E39" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="F39" t="s" s="19">
+      <c r="B40" t="s" s="22">
         <v>66</v>
       </c>
-      <c r="G39" s="3"/>
-    </row>
-    <row r="40" ht="13.65" customHeight="1">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="C40" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D40" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s" s="22">
+        <v>67</v>
+      </c>
       <c r="G40" s="3"/>
     </row>
     <row r="41" ht="13.65" customHeight="1">
-      <c r="A41" t="s" s="23">
-        <v>67</v>
-      </c>
+      <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -2487,38 +2499,38 @@
       <c r="G41" s="3"/>
     </row>
     <row r="42" ht="13.65" customHeight="1">
-      <c r="A42" t="s" s="19">
+      <c r="A42" t="s" s="26">
         <v>68</v>
       </c>
-      <c r="B42" t="s" s="19">
-        <v>69</v>
-      </c>
-      <c r="C42" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D42" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E42" t="s" s="19">
-        <v>13</v>
-      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
     </row>
     <row r="43" ht="13.65" customHeight="1">
-      <c r="A43" s="3"/>
-      <c r="B43" t="s" s="19">
+      <c r="A43" t="s" s="22">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s" s="22">
         <v>70</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="C43" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s" s="22">
+        <v>13</v>
+      </c>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" ht="13.65" customHeight="1">
       <c r="A44" s="3"/>
-      <c r="B44" t="s" s="19">
+      <c r="B44" t="s" s="22">
         <v>71</v>
       </c>
       <c r="C44" s="3"/>
@@ -2529,7 +2541,7 @@
     </row>
     <row r="45" ht="13.65" customHeight="1">
       <c r="A45" s="3"/>
-      <c r="B45" t="s" s="19">
+      <c r="B45" t="s" s="22">
         <v>72</v>
       </c>
       <c r="C45" s="3"/>
@@ -2540,7 +2552,7 @@
     </row>
     <row r="46" ht="13.65" customHeight="1">
       <c r="A46" s="3"/>
-      <c r="B46" t="s" s="19">
+      <c r="B46" t="s" s="22">
         <v>73</v>
       </c>
       <c r="C46" s="3"/>
@@ -2551,48 +2563,59 @@
     </row>
     <row r="47" ht="13.65" customHeight="1">
       <c r="A47" s="3"/>
-      <c r="B47" t="s" s="19">
+      <c r="B47" t="s" s="22">
         <v>74</v>
       </c>
-      <c r="C47" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D47" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E47" t="s" s="19">
-        <v>13</v>
-      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
     </row>
     <row r="48" ht="13.65" customHeight="1">
-      <c r="A48" t="s" s="19">
+      <c r="A48" s="3"/>
+      <c r="B48" t="s" s="22">
         <v>75</v>
       </c>
-      <c r="B48" t="s" s="19">
-        <v>76</v>
-      </c>
-      <c r="C48" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="D48" t="s" s="19">
-        <v>13</v>
-      </c>
-      <c r="E48" t="s" s="19">
+      <c r="C48" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D48" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E48" t="s" s="22">
         <v>13</v>
       </c>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" ht="13.65" customHeight="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="A49" t="s" s="22">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s" s="22">
+        <v>77</v>
+      </c>
+      <c r="C49" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E49" t="s" s="22">
+        <v>13</v>
+      </c>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
+    </row>
+    <row r="50" ht="13.65" customHeight="1">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2615,16 +2638,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.5" style="25" customWidth="1"/>
-    <col min="2" max="2" width="43.8516" style="25" customWidth="1"/>
-    <col min="3" max="3" width="40.1719" style="25" customWidth="1"/>
-    <col min="4" max="6" width="9.35156" style="25" customWidth="1"/>
-    <col min="7" max="256" width="11.8516" style="25" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="28" customWidth="1"/>
+    <col min="2" max="2" width="43.8516" style="28" customWidth="1"/>
+    <col min="3" max="3" width="40.1719" style="28" customWidth="1"/>
+    <col min="4" max="6" width="9.35156" style="28" customWidth="1"/>
+    <col min="7" max="256" width="11.8516" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.1" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2633,82 +2656,82 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="27">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s" s="28">
+      <c r="A3" t="s" s="30">
         <v>79</v>
       </c>
-      <c r="C3" t="s" s="28">
+      <c r="B3" t="s" s="31">
         <v>80</v>
       </c>
-      <c r="D3" t="s" s="29">
+      <c r="C3" t="s" s="31">
         <v>81</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="D3" t="s" s="32">
+        <v>82</v>
+      </c>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" t="s" s="28">
-        <v>82</v>
-      </c>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" t="s" s="31">
+        <v>83</v>
+      </c>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="33">
-        <v>83</v>
-      </c>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+      <c r="A5" t="s" s="36">
+        <v>84</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="35">
-        <v>84</v>
-      </c>
-      <c r="B6" t="s" s="35">
+      <c r="A6" t="s" s="18">
         <v>85</v>
       </c>
-      <c r="C6" t="s" s="35">
+      <c r="B6" t="s" s="18">
         <v>86</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" t="s" s="37">
+      <c r="C6" t="s" s="18">
         <v>87</v>
       </c>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" t="s" s="39">
+        <v>88</v>
+      </c>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" t="s" s="35">
-        <v>88</v>
-      </c>
-      <c r="B7" t="s" s="35">
+      <c r="A7" t="s" s="18">
         <v>89</v>
       </c>
-      <c r="C7" t="s" s="35">
+      <c r="B7" t="s" s="18">
         <v>90</v>
       </c>
-      <c r="D7" t="s" s="37">
+      <c r="C7" t="s" s="18">
         <v>91</v>
       </c>
-      <c r="E7" s="36">
+      <c r="D7" t="s" s="39">
+        <v>92</v>
+      </c>
+      <c r="E7" s="38">
         <v>150</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="38">
         <v>1256</v>
       </c>
     </row>
@@ -2716,15 +2739,15 @@
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" t="s" s="12">
-        <v>92</v>
-      </c>
-      <c r="D8" s="38">
+        <v>93</v>
+      </c>
+      <c r="D8" s="40">
         <v>-20</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="40">
         <v>6000</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8" s="40">
         <v>200</v>
       </c>
     </row>
@@ -2732,61 +2755,61 @@
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" t="s" s="15">
-        <v>93</v>
-      </c>
-      <c r="D9" s="39">
+        <v>94</v>
+      </c>
+      <c r="D9" s="41">
         <v>56.69</v>
       </c>
-      <c r="E9" t="s" s="40">
-        <v>94</v>
-      </c>
-      <c r="F9" s="39">
+      <c r="E9" t="s" s="42">
+        <v>95</v>
+      </c>
+      <c r="F9" s="41">
         <v>8000.65</v>
       </c>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" t="s" s="41">
-        <v>95</v>
-      </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="A10" t="s" s="17">
+        <v>96</v>
+      </c>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
       <c r="A11" t="s" s="12">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s" s="12">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s" s="12">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s" s="43">
-        <v>98</v>
-      </c>
-      <c r="E11" s="38">
+        <v>91</v>
+      </c>
+      <c r="D11" t="s" s="44">
+        <v>99</v>
+      </c>
+      <c r="E11" s="40">
         <v>150</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11" s="40">
         <v>12</v>
       </c>
     </row>
     <row r="12" ht="13.65" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
-      <c r="C12" t="s" s="19">
-        <v>99</v>
-      </c>
-      <c r="D12" s="44">
+      <c r="C12" t="s" s="22">
+        <v>100</v>
+      </c>
+      <c r="D12" s="45">
         <v>121</v>
       </c>
-      <c r="E12" s="44">
+      <c r="E12" s="45">
         <v>120</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="45">
         <v>7</v>
       </c>
     </row>
@@ -2794,97 +2817,97 @@
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" t="s" s="15">
-        <v>93</v>
-      </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
+        <v>94</v>
+      </c>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
       <c r="A14" t="s" s="12">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B14" t="s" s="12">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s" s="12">
-        <v>102</v>
-      </c>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" t="s" s="43">
         <v>103</v>
+      </c>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" t="s" s="44">
+        <v>104</v>
       </c>
     </row>
     <row r="15" ht="13.65" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" t="s" s="15">
-        <v>104</v>
-      </c>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" t="s" s="40">
         <v>105</v>
       </c>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" t="s" s="42">
+        <v>106</v>
+      </c>
     </row>
     <row r="16" ht="13.65" customHeight="1">
-      <c r="A16" t="s" s="41">
-        <v>106</v>
-      </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="A16" t="s" s="17">
+        <v>107</v>
+      </c>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
-      <c r="A17" t="s" s="35">
-        <v>107</v>
-      </c>
-      <c r="B17" t="s" s="35">
+      <c r="A17" t="s" s="18">
         <v>108</v>
       </c>
-      <c r="C17" t="s" s="35">
+      <c r="B17" t="s" s="18">
         <v>109</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
+      <c r="C17" t="s" s="18">
+        <v>110</v>
+      </c>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
       <c r="A18" t="s" s="12">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s" s="12">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C18" t="s" s="12">
-        <v>90</v>
-      </c>
-      <c r="D18" t="s" s="43">
-        <v>112</v>
-      </c>
-      <c r="E18" s="38">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s" s="44">
+        <v>113</v>
+      </c>
+      <c r="E18" s="40">
         <v>80</v>
       </c>
-      <c r="F18" s="38">
+      <c r="F18" s="40">
         <v>120</v>
       </c>
     </row>
     <row r="19" ht="13.65" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" t="s" s="19">
-        <v>113</v>
-      </c>
-      <c r="D19" s="44">
+      <c r="C19" t="s" s="22">
+        <v>114</v>
+      </c>
+      <c r="D19" s="45">
         <v>9</v>
       </c>
-      <c r="E19" s="44">
+      <c r="E19" s="45">
         <v>361</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="45">
         <v>360</v>
       </c>
     </row>
@@ -2892,32 +2915,32 @@
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" t="s" s="15">
-        <v>93</v>
-      </c>
-      <c r="D20" s="39">
+        <v>94</v>
+      </c>
+      <c r="D20" s="41">
         <v>45.6</v>
       </c>
-      <c r="E20" s="39">
+      <c r="E20" s="41">
         <v>800.6</v>
       </c>
-      <c r="F20" t="s" s="40">
-        <v>114</v>
+      <c r="F20" t="s" s="42">
+        <v>115</v>
       </c>
     </row>
     <row r="21" ht="13.15" customHeight="1">
       <c r="A21" t="s" s="12">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B21" t="s" s="12">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C21" t="s" s="12">
-        <v>117</v>
-      </c>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" t="s" s="43">
         <v>118</v>
+      </c>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" t="s" s="44">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test to iReadMore-texting.xlsx for the tabs
</commit_message>
<xml_diff>
--- a/attachments/iReadMore-testing.xlsx
+++ b/attachments/iReadMore-testing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>Testing of iReadMore WebApp</t>
   </si>
@@ -110,9 +110,15 @@
     <t>2. Checked that the values are right:</t>
   </si>
   <si>
+    <t>I changed the sample values later in the project,</t>
+  </si>
+  <si>
     <t xml:space="preserve">   a) Book-title: „Example“</t>
   </si>
   <si>
+    <t>Therefore they don’t correspond to the page now</t>
+  </si>
+  <si>
     <t xml:space="preserve">   b) Total number of pages: 120</t>
   </si>
   <si>
@@ -152,13 +158,22 @@
     <t xml:space="preserve">   c) Showing a calendar with 5 days circled</t>
   </si>
   <si>
+    <t>2. Toggling between tabs „Month“ and „Schedule“</t>
+  </si>
+  <si>
+    <t>Color theme of the tab corresponds to the normal buttons after tapping</t>
+  </si>
+  <si>
+    <t>Created new class „.btn-tab“ to avoid style conflict with the regular buttons</t>
+  </si>
+  <si>
     <t>Check output actions</t>
   </si>
   <si>
     <t xml:space="preserve">  a) Print View</t>
   </si>
   <si>
-    <t>Clicked on „Print View“ button</t>
+    <t>Clicked on „Print“ button after selecting the Schedule-tap</t>
   </si>
   <si>
     <t xml:space="preserve">Shows all pages to print, and not just one div. </t>
@@ -170,7 +185,7 @@
     <t xml:space="preserve">  b) Export to Google Calendar</t>
   </si>
   <si>
-    <t>Clicked on „Export“ button, checked that the following happens:</t>
+    <t>Clicked on „Export“ button in Month-tab, checked that the following happens:</t>
   </si>
   <si>
     <t>1. User prompted to Google login, followed steps</t>
@@ -612,7 +627,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -683,6 +698,12 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1835,7 +1856,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2011,9 +2032,11 @@
       <c r="G11" s="3"/>
     </row>
     <row r="12" ht="13.65" customHeight="1">
-      <c r="A12" s="3"/>
+      <c r="A12" t="s" s="23">
+        <v>24</v>
+      </c>
       <c r="B12" t="s" s="22">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s" s="22">
         <v>13</v>
@@ -2028,9 +2051,11 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" ht="13.65" customHeight="1">
-      <c r="A13" s="3"/>
+      <c r="A13" t="s" s="23">
+        <v>26</v>
+      </c>
       <c r="B13" t="s" s="22">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s" s="22">
         <v>13</v>
@@ -2047,7 +2072,7 @@
     <row r="14" ht="13.65" customHeight="1">
       <c r="A14" s="3"/>
       <c r="B14" t="s" s="22">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s" s="22">
         <v>13</v>
@@ -2064,7 +2089,7 @@
     <row r="15" ht="13.65" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" t="s" s="22">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s" s="22">
         <v>13</v>
@@ -2081,7 +2106,7 @@
     <row r="16" ht="13.65" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" t="s" s="22">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s" s="22">
         <v>13</v>
@@ -2098,7 +2123,7 @@
     <row r="17" ht="13.65" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" t="s" s="22">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s" s="22">
         <v>13</v>
@@ -2115,7 +2140,7 @@
     <row r="18" ht="13.65" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" t="s" s="15">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s" s="15">
         <v>13</v>
@@ -2131,10 +2156,10 @@
     </row>
     <row r="19" ht="13.65" customHeight="1">
       <c r="A19" t="s" s="12">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s" s="12">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13"/>
@@ -2145,7 +2170,7 @@
     <row r="20" ht="13.65" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" t="s" s="22">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s" s="22">
         <v>13</v>
@@ -2162,7 +2187,7 @@
     <row r="21" ht="13.65" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" t="s" s="22">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s" s="22">
         <v>13</v>
@@ -2170,18 +2195,18 @@
       <c r="D21" t="s" s="22">
         <v>13</v>
       </c>
-      <c r="E21" t="s" s="23">
-        <v>35</v>
+      <c r="E21" t="s" s="24">
+        <v>37</v>
       </c>
       <c r="F21" t="s" s="22">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" ht="13.65" customHeight="1">
       <c r="A22" s="14"/>
       <c r="B22" t="s" s="15">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s" s="15">
         <v>13</v>
@@ -2196,81 +2221,85 @@
       <c r="G22" s="14"/>
     </row>
     <row r="23" ht="13.65" customHeight="1">
-      <c r="A23" t="s" s="20">
+      <c r="A23" s="17"/>
+      <c r="B23" t="s" s="18">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s" s="18">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s" s="18">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s" s="25">
+        <v>16</v>
+      </c>
+      <c r="F23" t="s" s="18">
+        <v>41</v>
+      </c>
+      <c r="G23" t="s" s="18">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" ht="13.65" customHeight="1">
+      <c r="A24" t="s" s="20">
+        <v>43</v>
+      </c>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" ht="13.65" customHeight="1">
+      <c r="A25" t="s" s="15">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s" s="15">
+        <v>45</v>
+      </c>
+      <c r="C25" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s" s="16">
+        <v>16</v>
+      </c>
+      <c r="E25" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s" s="15">
+        <v>46</v>
+      </c>
+      <c r="G25" t="s" s="26">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" ht="13.65" customHeight="1">
+      <c r="A26" t="s" s="12">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s" s="12">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="D26" t="s" s="12">
+        <v>13</v>
+      </c>
+      <c r="E26" t="s" s="27">
+        <v>37</v>
+      </c>
+      <c r="F26" t="s" s="12">
         <v>38</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-    </row>
-    <row r="24" ht="13.65" customHeight="1">
-      <c r="A24" t="s" s="15">
-        <v>39</v>
-      </c>
-      <c r="B24" t="s" s="15">
-        <v>40</v>
-      </c>
-      <c r="C24" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s" s="16">
-        <v>16</v>
-      </c>
-      <c r="E24" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="F24" t="s" s="15">
-        <v>41</v>
-      </c>
-      <c r="G24" t="s" s="24">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" ht="13.65" customHeight="1">
-      <c r="A25" t="s" s="12">
-        <v>43</v>
-      </c>
-      <c r="B25" t="s" s="12">
-        <v>44</v>
-      </c>
-      <c r="C25" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="D25" t="s" s="12">
-        <v>13</v>
-      </c>
-      <c r="E25" t="s" s="25">
-        <v>35</v>
-      </c>
-      <c r="F25" t="s" s="12">
-        <v>36</v>
-      </c>
-      <c r="G25" s="13"/>
-    </row>
-    <row r="26" ht="13.65" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" t="s" s="22">
-        <v>45</v>
-      </c>
-      <c r="C26" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="D26" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="E26" t="s" s="22">
-        <v>46</v>
-      </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="G26" s="13"/>
     </row>
     <row r="27" ht="13.65" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" t="s" s="22">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s" s="22">
         <v>13</v>
@@ -2279,7 +2308,7 @@
         <v>13</v>
       </c>
       <c r="E27" t="s" s="22">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -2287,7 +2316,7 @@
     <row r="28" ht="13.65" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" t="s" s="22">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s" s="22">
         <v>13</v>
@@ -2296,7 +2325,7 @@
         <v>13</v>
       </c>
       <c r="E28" t="s" s="22">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -2304,17 +2333,25 @@
     <row r="29" ht="13.65" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" t="s" s="22">
-        <v>49</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="C29" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D29" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s" s="22">
+        <v>51</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" ht="13.65" customHeight="1">
       <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
+      <c r="B30" t="s" s="22">
+        <v>54</v>
+      </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -2322,9 +2359,7 @@
       <c r="G30" s="3"/>
     </row>
     <row r="31" ht="13.65" customHeight="1">
-      <c r="A31" t="s" s="26">
-        <v>50</v>
-      </c>
+      <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2333,37 +2368,37 @@
       <c r="G31" s="3"/>
     </row>
     <row r="32" ht="13.65" customHeight="1">
-      <c r="A32" t="s" s="22">
-        <v>51</v>
-      </c>
-      <c r="B32" t="s" s="22">
-        <v>52</v>
-      </c>
-      <c r="C32" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="D32" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="E32" t="s" s="22">
-        <v>13</v>
-      </c>
+      <c r="A32" t="s" s="28">
+        <v>55</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" ht="13.65" customHeight="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="A33" t="s" s="22">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s" s="22">
+        <v>57</v>
+      </c>
+      <c r="C33" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D33" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s" s="22">
+        <v>13</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" ht="13.65" customHeight="1">
-      <c r="A34" t="s" s="26">
-        <v>53</v>
-      </c>
+      <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -2372,30 +2407,22 @@
       <c r="G34" s="3"/>
     </row>
     <row r="35" ht="13.65" customHeight="1">
-      <c r="A35" t="s" s="22">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s" s="22">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="D35" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="E35" t="s" s="22">
-        <v>13</v>
-      </c>
+      <c r="A35" t="s" s="28">
+        <v>58</v>
+      </c>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" ht="13.65" customHeight="1">
       <c r="A36" t="s" s="22">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s" s="22">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s" s="22">
         <v>13</v>
@@ -2411,10 +2438,10 @@
     </row>
     <row r="37" ht="13.65" customHeight="1">
       <c r="A37" t="s" s="22">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s" s="22">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s" s="22">
         <v>13</v>
@@ -2430,10 +2457,10 @@
     </row>
     <row r="38" ht="13.65" customHeight="1">
       <c r="A38" t="s" s="22">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B38" t="s" s="22">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C38" t="s" s="22">
         <v>13</v>
@@ -2449,10 +2476,10 @@
     </row>
     <row r="39" ht="13.65" customHeight="1">
       <c r="A39" t="s" s="22">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s" s="22">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s" s="22">
         <v>13</v>
@@ -2464,16 +2491,14 @@
         <v>13</v>
       </c>
       <c r="F39" s="3"/>
-      <c r="G39" t="s" s="27">
-        <v>64</v>
-      </c>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" ht="13.65" customHeight="1">
       <c r="A40" t="s" s="22">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s" s="22">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s" s="22">
         <v>13</v>
@@ -2484,24 +2509,34 @@
       <c r="E40" t="s" s="22">
         <v>13</v>
       </c>
-      <c r="F40" t="s" s="22">
-        <v>67</v>
-      </c>
-      <c r="G40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" t="s" s="29">
+        <v>69</v>
+      </c>
     </row>
     <row r="41" ht="13.65" customHeight="1">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="A41" t="s" s="22">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s" s="22">
+        <v>71</v>
+      </c>
+      <c r="C41" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D41" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s" s="22">
+        <v>72</v>
+      </c>
       <c r="G41" s="3"/>
     </row>
     <row r="42" ht="13.65" customHeight="1">
-      <c r="A42" t="s" s="26">
-        <v>68</v>
-      </c>
+      <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -2510,39 +2545,39 @@
       <c r="G42" s="3"/>
     </row>
     <row r="43" ht="13.65" customHeight="1">
-      <c r="A43" t="s" s="22">
-        <v>69</v>
-      </c>
-      <c r="B43" t="s" s="22">
-        <v>70</v>
-      </c>
-      <c r="C43" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="D43" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="E43" t="s" s="22">
-        <v>13</v>
-      </c>
+      <c r="A43" t="s" s="28">
+        <v>73</v>
+      </c>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
     <row r="44" ht="13.65" customHeight="1">
-      <c r="A44" s="3"/>
+      <c r="A44" t="s" s="22">
+        <v>74</v>
+      </c>
       <c r="B44" t="s" s="22">
-        <v>71</v>
-      </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="C44" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D44" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E44" t="s" s="22">
+        <v>13</v>
+      </c>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
     </row>
     <row r="45" ht="13.65" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" t="s" s="22">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -2553,7 +2588,7 @@
     <row r="46" ht="13.65" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" t="s" s="22">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -2564,7 +2599,7 @@
     <row r="47" ht="13.65" customHeight="1">
       <c r="A47" s="3"/>
       <c r="B47" t="s" s="22">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -2575,26 +2610,18 @@
     <row r="48" ht="13.65" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" t="s" s="22">
-        <v>75</v>
-      </c>
-      <c r="C48" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="D48" t="s" s="22">
-        <v>13</v>
-      </c>
-      <c r="E48" t="s" s="22">
-        <v>13</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
     </row>
     <row r="49" ht="13.65" customHeight="1">
-      <c r="A49" t="s" s="22">
-        <v>76</v>
-      </c>
+      <c r="A49" s="3"/>
       <c r="B49" t="s" s="22">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s" s="22">
         <v>13</v>
@@ -2609,13 +2636,32 @@
       <c r="G49" s="3"/>
     </row>
     <row r="50" ht="13.65" customHeight="1">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="A50" t="s" s="22">
+        <v>81</v>
+      </c>
+      <c r="B50" t="s" s="22">
+        <v>82</v>
+      </c>
+      <c r="C50" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="D50" t="s" s="22">
+        <v>13</v>
+      </c>
+      <c r="E50" t="s" s="22">
+        <v>13</v>
+      </c>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
+    </row>
+    <row r="51" ht="13.65" customHeight="1">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2638,16 +2684,16 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.8333" defaultRowHeight="12.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="24.5" style="28" customWidth="1"/>
-    <col min="2" max="2" width="43.8516" style="28" customWidth="1"/>
-    <col min="3" max="3" width="40.1719" style="28" customWidth="1"/>
-    <col min="4" max="6" width="9.35156" style="28" customWidth="1"/>
-    <col min="7" max="256" width="11.8516" style="28" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="30" customWidth="1"/>
+    <col min="2" max="2" width="43.8516" style="30" customWidth="1"/>
+    <col min="3" max="3" width="40.1719" style="30" customWidth="1"/>
+    <col min="4" max="6" width="9.35156" style="30" customWidth="1"/>
+    <col min="7" max="256" width="11.8516" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.1" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2656,82 +2702,82 @@
       <c r="F1" s="3"/>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="30">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s" s="31">
-        <v>80</v>
-      </c>
-      <c r="C3" t="s" s="31">
-        <v>81</v>
-      </c>
-      <c r="D3" t="s" s="32">
-        <v>82</v>
-      </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="34"/>
+      <c r="A3" t="s" s="32">
+        <v>84</v>
+      </c>
+      <c r="B3" t="s" s="33">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s" s="33">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s" s="34">
+        <v>87</v>
+      </c>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="35"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" t="s" s="31">
-        <v>83</v>
-      </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="34"/>
+      <c r="A4" s="37"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" t="s" s="33">
+        <v>88</v>
+      </c>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="36">
-        <v>84</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
+      <c r="A5" t="s" s="38">
+        <v>89</v>
+      </c>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
     </row>
     <row r="6" ht="13.65" customHeight="1">
       <c r="A6" t="s" s="18">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s" s="18">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s" s="18">
-        <v>87</v>
-      </c>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" t="s" s="39">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" t="s" s="41">
+        <v>93</v>
       </c>
     </row>
     <row r="7" ht="13.65" customHeight="1">
       <c r="A7" t="s" s="18">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s" s="18">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s" s="18">
-        <v>91</v>
-      </c>
-      <c r="D7" t="s" s="39">
-        <v>92</v>
-      </c>
-      <c r="E7" s="38">
+        <v>96</v>
+      </c>
+      <c r="D7" t="s" s="41">
+        <v>97</v>
+      </c>
+      <c r="E7" s="40">
         <v>150</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7" s="40">
         <v>1256</v>
       </c>
     </row>
@@ -2739,15 +2785,15 @@
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" t="s" s="12">
-        <v>93</v>
-      </c>
-      <c r="D8" s="40">
+        <v>98</v>
+      </c>
+      <c r="D8" s="42">
         <v>-20</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="42">
         <v>6000</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="42">
         <v>200</v>
       </c>
     </row>
@@ -2755,45 +2801,45 @@
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" t="s" s="15">
-        <v>94</v>
-      </c>
-      <c r="D9" s="41">
+        <v>99</v>
+      </c>
+      <c r="D9" s="43">
         <v>56.69</v>
       </c>
-      <c r="E9" t="s" s="42">
-        <v>95</v>
-      </c>
-      <c r="F9" s="41">
+      <c r="E9" t="s" s="44">
+        <v>100</v>
+      </c>
+      <c r="F9" s="43">
         <v>8000.65</v>
       </c>
     </row>
     <row r="10" ht="13.65" customHeight="1">
       <c r="A10" t="s" s="17">
-        <v>96</v>
-      </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+        <v>101</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" ht="13.65" customHeight="1">
       <c r="A11" t="s" s="12">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B11" t="s" s="12">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="C11" t="s" s="12">
-        <v>91</v>
-      </c>
-      <c r="D11" t="s" s="44">
-        <v>99</v>
-      </c>
-      <c r="E11" s="40">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s" s="46">
+        <v>104</v>
+      </c>
+      <c r="E11" s="42">
         <v>150</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="42">
         <v>12</v>
       </c>
     </row>
@@ -2801,15 +2847,15 @@
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" t="s" s="22">
-        <v>100</v>
-      </c>
-      <c r="D12" s="45">
+        <v>105</v>
+      </c>
+      <c r="D12" s="47">
         <v>121</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="47">
         <v>120</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="47">
         <v>7</v>
       </c>
     </row>
@@ -2817,81 +2863,81 @@
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" t="s" s="15">
-        <v>94</v>
-      </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+        <v>99</v>
+      </c>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" ht="13.65" customHeight="1">
       <c r="A14" t="s" s="12">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s" s="12">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s" s="12">
-        <v>103</v>
-      </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" t="s" s="44">
-        <v>104</v>
+        <v>108</v>
+      </c>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" t="s" s="46">
+        <v>109</v>
       </c>
     </row>
     <row r="15" ht="13.65" customHeight="1">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" t="s" s="15">
-        <v>105</v>
-      </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" t="s" s="42">
-        <v>106</v>
+        <v>110</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" t="s" s="44">
+        <v>111</v>
       </c>
     </row>
     <row r="16" ht="13.65" customHeight="1">
       <c r="A16" t="s" s="17">
-        <v>107</v>
-      </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+        <v>112</v>
+      </c>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
     </row>
     <row r="17" ht="13.65" customHeight="1">
       <c r="A17" t="s" s="18">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B17" t="s" s="18">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s" s="18">
-        <v>110</v>
-      </c>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+        <v>115</v>
+      </c>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
     </row>
     <row r="18" ht="13.65" customHeight="1">
       <c r="A18" t="s" s="12">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B18" t="s" s="12">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s" s="12">
-        <v>91</v>
-      </c>
-      <c r="D18" t="s" s="44">
-        <v>113</v>
-      </c>
-      <c r="E18" s="40">
+        <v>96</v>
+      </c>
+      <c r="D18" t="s" s="46">
+        <v>118</v>
+      </c>
+      <c r="E18" s="42">
         <v>80</v>
       </c>
-      <c r="F18" s="40">
+      <c r="F18" s="42">
         <v>120</v>
       </c>
     </row>
@@ -2899,15 +2945,15 @@
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s" s="22">
-        <v>114</v>
-      </c>
-      <c r="D19" s="45">
+        <v>119</v>
+      </c>
+      <c r="D19" s="47">
         <v>9</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="47">
         <v>361</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="47">
         <v>360</v>
       </c>
     </row>
@@ -2915,32 +2961,32 @@
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" t="s" s="15">
-        <v>94</v>
-      </c>
-      <c r="D20" s="41">
+        <v>99</v>
+      </c>
+      <c r="D20" s="43">
         <v>45.6</v>
       </c>
-      <c r="E20" s="41">
+      <c r="E20" s="43">
         <v>800.6</v>
       </c>
-      <c r="F20" t="s" s="42">
-        <v>115</v>
+      <c r="F20" t="s" s="44">
+        <v>120</v>
       </c>
     </row>
     <row r="21" ht="13.15" customHeight="1">
       <c r="A21" t="s" s="12">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="B21" t="s" s="12">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s" s="12">
-        <v>118</v>
-      </c>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
-      <c r="F21" t="s" s="44">
-        <v>119</v>
+        <v>123</v>
+      </c>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" t="s" s="46">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>